<commit_message>
Vitamine in can, automotization
</commit_message>
<xml_diff>
--- a/data/energy.xlsx
+++ b/data/energy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\EnergyExplorer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F375948C-CEBB-44BB-A6D8-5302423EC5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CBE6A3-D70E-4401-91B9-8120650696D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E063C6F-A15E-437B-9958-F28241C4B78E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E063C6F-A15E-437B-9958-F28241C4B78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
   <si>
     <t>id</t>
   </si>
@@ -47,9 +47,6 @@
     <t>company</t>
   </si>
   <si>
-    <t>carbohydrates</t>
-  </si>
-  <si>
     <t>calories</t>
   </si>
   <si>
@@ -242,15 +239,9 @@
     <t>caffeine</t>
   </si>
   <si>
-    <t>caffeine_in_can</t>
-  </si>
-  <si>
     <t>Кофеин</t>
   </si>
   <si>
-    <t>sugar_in_can</t>
-  </si>
-  <si>
     <t>Сахар</t>
   </si>
   <si>
@@ -270,6 +261,9 @@
   </si>
   <si>
     <t>Пантотеновая кислота</t>
+  </si>
+  <si>
+    <t>sugar</t>
   </si>
 </sst>
 </file>
@@ -632,7 +626,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,55 +645,55 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -707,39 +701,39 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2">
+        <v>480</v>
+      </c>
+      <c r="F2" s="2">
+        <f>E2/I2*100</f>
+        <v>106.90423162583519</v>
+      </c>
+      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="I2">
+        <f>H2*1000</f>
+        <v>449</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>10.5</v>
       </c>
-      <c r="E2">
+      <c r="L2">
         <v>34</v>
-      </c>
-      <c r="F2">
-        <v>120</v>
-      </c>
-      <c r="G2">
-        <v>480</v>
-      </c>
-      <c r="H2" s="2">
-        <f>G2/K2*100</f>
-        <v>106.90423162583519</v>
-      </c>
-      <c r="I2">
-        <v>42</v>
-      </c>
-      <c r="J2">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="K2">
-        <f>J2*1000</f>
-        <v>449</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
       </c>
       <c r="M2" s="1">
         <v>3.4</v>
@@ -759,73 +753,73 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3">
+        <v>240</v>
+      </c>
+      <c r="E3">
+        <v>480</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F31" si="0">E3/I3*100</f>
+        <v>106.90423162583519</v>
+      </c>
+      <c r="G3">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I31" si="1">H3*1000</f>
+        <v>449</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>12.5</v>
       </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>240</v>
-      </c>
-      <c r="G3">
-        <v>480</v>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H31" si="0">G3/K3*100</f>
-        <v>106.90423162583519</v>
-      </c>
-      <c r="I3">
-        <v>54</v>
-      </c>
-      <c r="J3">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K31" si="1">J3*1000</f>
-        <v>449</v>
-      </c>
       <c r="L3">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4">
+        <v>120</v>
+      </c>
+      <c r="E4">
+        <v>316</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>126.4</v>
+      </c>
+      <c r="G4">
+        <v>44</v>
+      </c>
+      <c r="H4">
+        <v>0.25</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K4">
         <v>10.5</v>
       </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>120</v>
-      </c>
-      <c r="G4">
-        <v>316</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>126.4</v>
-      </c>
-      <c r="I4">
-        <v>44</v>
-      </c>
-      <c r="J4">
-        <v>0.25</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>250</v>
+      <c r="L4">
+        <v>30</v>
       </c>
       <c r="M4" s="1">
         <v>3.4</v>
@@ -845,36 +839,36 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>12.5</v>
       </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>34</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>50</v>
-      </c>
-      <c r="J5">
-        <v>0.5</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>500</v>
-      </c>
       <c r="L5">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -882,36 +876,36 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>0.33</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>11.2</v>
       </c>
-      <c r="E6">
-        <v>30</v>
-      </c>
-      <c r="F6">
-        <v>32</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>50</v>
-      </c>
-      <c r="J6">
-        <v>0.33</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>330</v>
-      </c>
       <c r="L6">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -919,36 +913,36 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>26</v>
+      </c>
+      <c r="H7">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>449</v>
+      </c>
+      <c r="J7">
+        <v>40</v>
+      </c>
+      <c r="K7">
         <v>6.9</v>
       </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>26</v>
-      </c>
-      <c r="J7">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>449</v>
-      </c>
       <c r="L7">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -956,36 +950,36 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8">
+        <v>44</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>28</v>
+      </c>
+      <c r="H8">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>449</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>7</v>
       </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>44</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>28</v>
-      </c>
-      <c r="J8">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>449</v>
-      </c>
       <c r="L8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M8" s="1">
         <v>3</v>
@@ -1002,36 +996,36 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>43</v>
+      </c>
+      <c r="H9">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>449</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>10.5</v>
       </c>
-      <c r="E9">
-        <v>30</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>43</v>
-      </c>
-      <c r="J9">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>449</v>
-      </c>
       <c r="L9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M9" s="1">
         <v>2.16</v>
@@ -1048,33 +1042,33 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>0.7</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="K10">
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="L10">
         <v>32</v>
-      </c>
-      <c r="F10">
-        <v>30</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>50</v>
-      </c>
-      <c r="J10">
-        <v>0.7</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>700</v>
       </c>
       <c r="M10" s="1">
         <v>6</v>
@@ -1091,33 +1085,33 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>0.7</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="K11">
         <v>12</v>
       </c>
-      <c r="E11">
-        <v>30</v>
-      </c>
-      <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>50</v>
-      </c>
-      <c r="J11">
-        <v>0.7</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>700</v>
+      <c r="L11">
+        <v>30</v>
       </c>
       <c r="M11" s="1">
         <v>6.4</v>
@@ -1134,33 +1128,33 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
       <c r="D12">
+        <v>26</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <v>0.7</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="K12">
         <v>10.5</v>
       </c>
-      <c r="E12">
+      <c r="L12">
         <v>28</v>
-      </c>
-      <c r="F12">
-        <v>26</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>45</v>
-      </c>
-      <c r="J12">
-        <v>0.7</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>700</v>
       </c>
       <c r="M12" s="1">
         <v>6.8</v>
@@ -1183,37 +1177,37 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
       <c r="D13">
+        <v>120</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>0.45</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J13">
+        <v>10.64</v>
+      </c>
+      <c r="K13">
         <v>12</v>
       </c>
-      <c r="E13">
+      <c r="L13">
         <f>117.5/4.5</f>
         <v>26.111111111111111</v>
-      </c>
-      <c r="F13">
-        <v>120</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>50</v>
-      </c>
-      <c r="J13">
-        <v>0.45</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="L13">
-        <v>10.64</v>
       </c>
       <c r="M13" s="1">
         <f>26.6/4.5</f>
@@ -1239,39 +1233,39 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14">
+        <v>120</v>
+      </c>
+      <c r="E14">
+        <v>290</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>64.444444444444443</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>0.45</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14">
         <v>12.5</v>
       </c>
-      <c r="E14">
+      <c r="L14">
         <v>27</v>
-      </c>
-      <c r="F14">
-        <v>120</v>
-      </c>
-      <c r="G14">
-        <v>290</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>64.444444444444443</v>
-      </c>
-      <c r="I14">
-        <v>50</v>
-      </c>
-      <c r="J14">
-        <v>0.45</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="L14">
-        <v>6</v>
       </c>
       <c r="M14" s="1">
         <v>6</v>
@@ -1294,39 +1288,39 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15">
+        <v>266</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>59.111111111111114</v>
+      </c>
+      <c r="G15">
+        <v>45</v>
+      </c>
+      <c r="H15">
+        <v>0.45</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J15">
+        <v>3.3</v>
+      </c>
+      <c r="K15">
         <v>11</v>
       </c>
-      <c r="E15">
+      <c r="L15">
         <v>27</v>
-      </c>
-      <c r="F15">
-        <v>120</v>
-      </c>
-      <c r="G15">
-        <v>266</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>59.111111111111114</v>
-      </c>
-      <c r="I15">
-        <v>45</v>
-      </c>
-      <c r="J15">
-        <v>0.45</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="L15">
-        <v>3.3</v>
       </c>
       <c r="M15" s="1">
         <v>3.3</v>
@@ -1352,39 +1346,39 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16">
+        <v>33</v>
+      </c>
+      <c r="E16">
+        <v>290</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>64.444444444444443</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>0.45</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
         <v>12.5</v>
       </c>
-      <c r="E16">
+      <c r="L16">
         <v>34</v>
-      </c>
-      <c r="F16">
-        <v>33</v>
-      </c>
-      <c r="G16">
-        <v>290</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="0"/>
-        <v>64.444444444444443</v>
-      </c>
-      <c r="I16">
-        <v>50</v>
-      </c>
-      <c r="J16">
-        <v>0.45</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="L16">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -1392,39 +1386,39 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
       <c r="D17">
+        <v>240</v>
+      </c>
+      <c r="E17">
+        <v>311</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>62.2</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>12</v>
       </c>
-      <c r="E17">
-        <v>30</v>
-      </c>
-      <c r="F17">
-        <v>240</v>
-      </c>
-      <c r="G17">
-        <v>311</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>62.2</v>
-      </c>
-      <c r="I17">
-        <v>50</v>
-      </c>
-      <c r="J17">
-        <v>0.5</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>500</v>
-      </c>
       <c r="L17">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -1432,73 +1426,73 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18">
+        <v>34</v>
+      </c>
+      <c r="E18">
+        <v>311</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>62.2</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>12.5</v>
       </c>
-      <c r="E18">
-        <v>30</v>
-      </c>
-      <c r="F18">
-        <v>34</v>
-      </c>
-      <c r="G18">
-        <v>311</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>62.2</v>
-      </c>
-      <c r="I18">
-        <v>50</v>
-      </c>
-      <c r="J18">
-        <v>0.5</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>500</v>
-      </c>
       <c r="L18">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>325</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>72.222222222222214</v>
+      </c>
+      <c r="G19">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>0.45</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="K19">
         <v>12</v>
       </c>
-      <c r="E19">
-        <v>30</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>325</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
-        <v>72.222222222222214</v>
-      </c>
-      <c r="I19">
-        <v>50</v>
-      </c>
-      <c r="J19">
-        <v>0.45</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>450</v>
+      <c r="L19">
+        <v>30</v>
       </c>
       <c r="M19" s="1">
         <v>2.88</v>
@@ -1524,39 +1518,39 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>317</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>70.444444444444443</v>
+      </c>
+      <c r="G20">
+        <v>54</v>
+      </c>
+      <c r="H20">
+        <v>0.45</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
         <v>13.5</v>
       </c>
-      <c r="E20">
-        <v>30</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>317</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="0"/>
-        <v>70.444444444444443</v>
-      </c>
-      <c r="I20">
-        <v>54</v>
-      </c>
-      <c r="J20">
-        <v>0.45</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
       <c r="L20">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O20" s="1">
         <v>0.75</v>
@@ -1576,39 +1570,39 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>317</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>70.444444444444443</v>
+      </c>
+      <c r="G21">
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <v>0.45</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
         <v>8</v>
       </c>
-      <c r="E21">
+      <c r="L21">
         <v>31</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>317</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>70.444444444444443</v>
-      </c>
-      <c r="I21">
-        <v>30</v>
-      </c>
-      <c r="J21">
-        <v>0.45</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
       </c>
       <c r="M21" s="1">
         <v>2.88</v>
@@ -1634,77 +1628,77 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22">
+        <f>400/2.5</f>
+        <v>160</v>
+      </c>
+      <c r="E22">
+        <v>480</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="G22">
+        <f>115/2.5</f>
+        <v>46</v>
+      </c>
+      <c r="H22">
+        <v>0.25</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="J22">
+        <f>28/2.5</f>
+        <v>11.2</v>
+      </c>
+      <c r="K22">
         <f>29/2.5</f>
         <v>11.6</v>
       </c>
-      <c r="E22">
+      <c r="L22">
         <v>24</v>
-      </c>
-      <c r="F22">
-        <f>400/2.5</f>
-        <v>160</v>
-      </c>
-      <c r="G22">
-        <v>480</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="0"/>
-        <v>192</v>
-      </c>
-      <c r="I22">
-        <f>115/2.5</f>
-        <v>46</v>
-      </c>
-      <c r="J22">
-        <v>0.25</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>250</v>
-      </c>
-      <c r="L22">
-        <f>28/2.5</f>
-        <v>11.2</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23">
+        <v>400</v>
+      </c>
+      <c r="E23">
+        <v>493</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>197.2</v>
+      </c>
+      <c r="G23">
+        <v>45</v>
+      </c>
+      <c r="H23">
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K23">
         <v>11</v>
       </c>
-      <c r="E23">
-        <v>30</v>
-      </c>
-      <c r="F23">
-        <v>400</v>
-      </c>
-      <c r="G23">
-        <v>493</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="0"/>
-        <v>197.2</v>
-      </c>
-      <c r="I23">
-        <v>45</v>
-      </c>
-      <c r="J23">
-        <v>0.25</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>250</v>
+      <c r="L23">
+        <v>30</v>
       </c>
       <c r="M23" s="1">
         <v>8</v>
@@ -1721,36 +1715,36 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
         <v>61</v>
       </c>
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
       <c r="D24">
+        <v>400</v>
+      </c>
+      <c r="E24">
+        <v>493</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>197.2</v>
+      </c>
+      <c r="G24">
+        <v>45</v>
+      </c>
+      <c r="H24">
+        <v>0.25</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K24">
         <v>11</v>
       </c>
-      <c r="E24">
-        <v>30</v>
-      </c>
-      <c r="F24">
-        <v>400</v>
-      </c>
-      <c r="G24">
-        <v>493</v>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" si="0"/>
-        <v>197.2</v>
-      </c>
-      <c r="I24">
-        <v>45</v>
-      </c>
-      <c r="J24">
-        <v>0.25</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="1"/>
-        <v>250</v>
+      <c r="L24">
+        <v>30</v>
       </c>
       <c r="M24" s="1">
         <v>8</v>
@@ -1767,36 +1761,36 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25">
+        <v>400</v>
+      </c>
+      <c r="E25">
+        <v>493</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>197.2</v>
+      </c>
+      <c r="G25">
+        <v>45</v>
+      </c>
+      <c r="H25">
+        <v>0.25</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K25">
         <v>11</v>
       </c>
-      <c r="E25">
-        <v>30</v>
-      </c>
-      <c r="F25">
-        <v>400</v>
-      </c>
-      <c r="G25">
-        <v>493</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="0"/>
-        <v>197.2</v>
-      </c>
-      <c r="I25">
-        <v>45</v>
-      </c>
-      <c r="J25">
-        <v>0.25</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="1"/>
-        <v>250</v>
+      <c r="L25">
+        <v>30</v>
       </c>
       <c r="M25" s="1">
         <v>8</v>
@@ -1816,39 +1810,39 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>333</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>66.600000000000009</v>
+      </c>
+      <c r="G26">
+        <v>51</v>
+      </c>
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
         <v>13</v>
       </c>
-      <c r="E26">
-        <v>30</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>333</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="0"/>
-        <v>66.600000000000009</v>
-      </c>
-      <c r="I26">
-        <v>51</v>
-      </c>
-      <c r="J26">
-        <v>0.5</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="1"/>
-        <v>500</v>
-      </c>
       <c r="L26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M26" s="1">
         <v>1.8</v>
@@ -1871,36 +1865,36 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27">
+        <v>200</v>
+      </c>
+      <c r="E27">
+        <v>223</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="0"/>
+        <v>44.6</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>0.5</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="K27">
         <v>12</v>
       </c>
-      <c r="E27">
-        <v>30</v>
-      </c>
-      <c r="F27">
-        <v>200</v>
-      </c>
-      <c r="G27">
-        <v>223</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="0"/>
-        <v>44.6</v>
-      </c>
-      <c r="I27">
-        <v>50</v>
-      </c>
-      <c r="J27">
-        <v>0.5</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="1"/>
-        <v>500</v>
+      <c r="L27">
+        <v>30</v>
       </c>
       <c r="M27" s="1">
         <v>1.9</v>
@@ -1923,39 +1917,39 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28">
+        <v>40</v>
+      </c>
+      <c r="E28">
+        <v>317</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>70.444444444444443</v>
+      </c>
+      <c r="G28">
+        <v>45</v>
+      </c>
+      <c r="H28">
+        <v>0.45</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
         <v>10.9</v>
       </c>
-      <c r="E28">
-        <v>30</v>
-      </c>
-      <c r="F28">
-        <v>40</v>
-      </c>
-      <c r="G28">
-        <v>317</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>70.444444444444443</v>
-      </c>
-      <c r="I28">
-        <v>45</v>
-      </c>
-      <c r="J28">
-        <v>0.45</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
       <c r="L28">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M28" s="1">
         <v>1.1000000000000001</v>
@@ -1975,39 +1969,39 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
         <v>14</v>
       </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
       <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>301</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="0"/>
+        <v>66.888888888888886</v>
+      </c>
+      <c r="G29">
+        <v>41</v>
+      </c>
+      <c r="H29">
+        <v>0.45</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
         <v>10.1</v>
       </c>
-      <c r="E29">
-        <v>30</v>
-      </c>
-      <c r="F29">
-        <v>40</v>
-      </c>
-      <c r="G29">
-        <v>301</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="0"/>
-        <v>66.888888888888886</v>
-      </c>
-      <c r="I29">
-        <v>41</v>
-      </c>
-      <c r="J29">
-        <v>0.45</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
       <c r="L29">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2015,39 +2009,39 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
         <v>27</v>
       </c>
-      <c r="C30" t="s">
-        <v>28</v>
-      </c>
       <c r="D30">
+        <v>199.5</v>
+      </c>
+      <c r="E30">
+        <v>347</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="0"/>
+        <v>77.111111111111114</v>
+      </c>
+      <c r="G30">
+        <v>51</v>
+      </c>
+      <c r="H30">
+        <v>0.45</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
         <v>12.7</v>
       </c>
-      <c r="E30">
-        <v>30</v>
-      </c>
-      <c r="F30">
-        <v>199.5</v>
-      </c>
-      <c r="G30">
-        <v>347</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>77.111111111111114</v>
-      </c>
-      <c r="I30">
-        <v>51</v>
-      </c>
-      <c r="J30">
-        <v>0.45</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
       <c r="L30">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M30" s="1">
         <v>1.68</v>
@@ -2073,39 +2067,39 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <v>371</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="0"/>
+        <v>82.444444444444443</v>
+      </c>
+      <c r="G31">
+        <v>48</v>
+      </c>
+      <c r="H31">
+        <v>0.45</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
         <v>12</v>
       </c>
-      <c r="E31">
-        <v>30</v>
-      </c>
-      <c r="F31">
-        <v>40</v>
-      </c>
-      <c r="G31">
-        <v>371</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="0"/>
-        <v>82.444444444444443</v>
-      </c>
-      <c r="I31">
-        <v>48</v>
-      </c>
-      <c r="J31">
-        <v>0.45</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
       <c r="L31">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M31" s="1">
         <v>1.44</v>
@@ -2138,163 +2132,163 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>1.5</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>1000</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>